<commit_message>
Last update before start
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_viz_MA/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D65D859-9E31-0C47-A874-B1A7F1510F64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41815900-5045-914E-95DD-17609731F618}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -120,9 +120,6 @@
     <t>Income · Geometries</t>
   </si>
   <si>
-    <t>Policy · Maps</t>
-  </si>
-  <si>
     <t>Round-up</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Mobility · Colors</t>
   </si>
   <si>
-    <t>Power · Themes</t>
-  </si>
-  <si>
     <t>lines</t>
   </si>
   <si>
@@ -145,6 +139,12 @@
   </si>
   <si>
     <t>dumbbell</t>
+  </si>
+  <si>
+    <t>Policy · Themes</t>
+  </si>
+  <si>
+    <t>Taxation · Maps</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,13 +653,13 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -673,7 +673,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -687,14 +687,14 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -722,13 +722,13 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H10">
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -770,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update syllabus and add slides
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_viz_MA/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41815900-5045-914E-95DD-17609731F618}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7518978D-4838-F541-961C-99EB24D8173D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -93,9 +93,6 @@
     <t>03_visualization.RData</t>
   </si>
   <si>
-    <t>10.30-12.30</t>
-  </si>
-  <si>
     <t>TC.4.02</t>
   </si>
   <si>
@@ -145,6 +142,30 @@
   </si>
   <si>
     <t>Taxation · Maps</t>
+  </si>
+  <si>
+    <t>10.30-12.00</t>
+  </si>
+  <si>
+    <t>04_income</t>
+  </si>
+  <si>
+    <t>04_income.R</t>
+  </si>
+  <si>
+    <t>04_income.RData</t>
+  </si>
+  <si>
+    <t>05_wealth</t>
+  </si>
+  <si>
+    <t>05_wealth.R</t>
+  </si>
+  <si>
+    <t>05_wealth.RData</t>
+  </si>
+  <si>
+    <t>06_mobility</t>
   </si>
 </sst>
 </file>
@@ -518,7 +539,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +588,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -581,10 +602,10 @@
         <v>45579</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -610,10 +631,10 @@
         <v>45586</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -639,7 +660,16 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -650,16 +680,25 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -670,10 +709,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -684,17 +726,17 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -705,10 +747,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -719,16 +761,16 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10">
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -753,7 +795,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -770,7 +812,7 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add slides for two sessions
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_viz_MA/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E672EA2E-794C-2041-81EF-B50A07355830}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771FE9AD-9FF7-8444-90CB-DC535EB3D461}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Income · Geometries</t>
   </si>
   <si>
-    <t>Round-up</t>
-  </si>
-  <si>
     <t>Growth · Labels</t>
   </si>
   <si>
@@ -193,6 +190,18 @@
   </si>
   <si>
     <t>09_policy</t>
+  </si>
+  <si>
+    <t>09_policy.R</t>
+  </si>
+  <si>
+    <t>09_policy.RData</t>
+  </si>
+  <si>
+    <t>Hackathon</t>
+  </si>
+  <si>
+    <t>10_hackathon</t>
   </si>
 </sst>
 </file>
@@ -566,7 +575,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +638,7 @@
         <v>45579</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -658,7 +667,7 @@
         <v>45586</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -690,13 +699,13 @@
         <v>29</v>
       </c>
       <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -710,22 +719,22 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -739,16 +748,16 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -762,22 +771,22 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
         <v>48</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -791,16 +800,16 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>52</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>53</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -814,16 +823,22 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
         <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
       </c>
       <c r="H10">
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -865,7 +880,10 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>